<commit_message>
complete goals and data
</commit_message>
<xml_diff>
--- a/Data/Donanemab.xlsx
+++ b/Data/Donanemab.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Desktop\Master\P8105\Homework\Alzheimers_Disease_New_Hope\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B719022-85D4-4720-B2D4-6D5CE2C9006F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93789E61-4ABF-4DF4-80BC-168FAD77AC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10920" yWindow="0" windowWidth="11109" windowHeight="11709" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" r:id="rId1"/>
-    <sheet name="AE" sheetId="2" r:id="rId2"/>
-    <sheet name="safety" sheetId="5" r:id="rId3"/>
-    <sheet name="K-M" sheetId="3" r:id="rId4"/>
-    <sheet name="result" sheetId="6" r:id="rId5"/>
+    <sheet name="AE" sheetId="2" r:id="rId1"/>
+    <sheet name="safety" sheetId="5" r:id="rId2"/>
+    <sheet name="K-M" sheetId="3" r:id="rId3"/>
+    <sheet name="result" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
   <si>
     <t>CDR-SB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -505,187 +504,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BECDFD9-8B14-40E0-BE81-5474177718C8}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
       <c r="B2">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>205</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>168</v>
+      </c>
+      <c r="C4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>114</v>
+      </c>
+      <c r="C6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <v>36</v>
-      </c>
-      <c r="F2">
-        <v>52</v>
-      </c>
-      <c r="G2">
-        <v>64</v>
-      </c>
-      <c r="H2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>546</v>
-      </c>
-      <c r="C3">
-        <v>530</v>
-      </c>
-      <c r="D3">
-        <v>499</v>
-      </c>
-      <c r="E3">
-        <v>471</v>
-      </c>
-      <c r="F3">
-        <v>451</v>
-      </c>
-      <c r="G3">
-        <v>418</v>
-      </c>
-      <c r="H3">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>569</v>
-      </c>
-      <c r="C4">
-        <v>561</v>
-      </c>
-      <c r="D4">
-        <v>540</v>
-      </c>
-      <c r="E4">
-        <v>516</v>
-      </c>
-      <c r="F4">
-        <v>486</v>
-      </c>
-      <c r="G4">
-        <v>461</v>
-      </c>
-      <c r="H4">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C5">
-        <f>(C3-B3)/B3</f>
-        <v>-2.9304029304029304E-2</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:E5" si="0">(D3-C3)/C3</f>
-        <v>-5.849056603773585E-2</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>-5.6112224448897796E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>24</v>
-      </c>
-      <c r="E8">
-        <v>36</v>
-      </c>
-      <c r="F8">
-        <v>52</v>
-      </c>
-      <c r="G8">
-        <v>64</v>
-      </c>
-      <c r="H8">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
       <c r="B9">
-        <v>533</v>
+        <v>53</v>
       </c>
       <c r="C9">
-        <v>517</v>
-      </c>
-      <c r="D9">
-        <v>487</v>
-      </c>
-      <c r="E9">
-        <v>459</v>
-      </c>
-      <c r="F9">
-        <v>441</v>
-      </c>
-      <c r="G9">
-        <v>406</v>
-      </c>
-      <c r="H9">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>560</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>549</v>
-      </c>
-      <c r="D10">
-        <v>526</v>
-      </c>
-      <c r="E10">
-        <v>506</v>
-      </c>
-      <c r="F10">
-        <v>474</v>
-      </c>
-      <c r="G10">
-        <v>447</v>
-      </c>
-      <c r="H10">
-        <v>444</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -695,132 +630,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BECDFD9-8B14-40E0-BE81-5474177718C8}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>74</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>205</v>
-      </c>
-      <c r="C3">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>168</v>
-      </c>
-      <c r="C4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>119</v>
-      </c>
-      <c r="C5">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>114</v>
-      </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>49</v>
-      </c>
-      <c r="C8">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>53</v>
-      </c>
-      <c r="C9">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>43</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945A234-0C75-4026-ABAA-5A9EB8483AF0}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -891,7 +700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B1883B-9163-4EFC-8E7E-B0A652D42AF0}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1145,11 +954,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660C716-DE70-4357-B0AE-9772EEE5742A}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>